<commit_message>
Atualizar arq. README, arq. ms-excel e inserir imagens png
</commit_message>
<xml_diff>
--- a/desafio_Ferramenta-de-Controle-de-Investimento_Santander-Excel-com-IA_DIO.xlsx
+++ b/desafio_Ferramenta-de-Controle-de-Investimento_Santander-Excel-com-IA_DIO.xlsx
@@ -76,7 +76,7 @@
     <t>PERFIL</t>
   </si>
   <si>
-    <t>Conservador</t>
+    <t>Moderado</t>
   </si>
   <si>
     <t>Investimento Mensal</t>
@@ -118,6 +118,9 @@
     <t>%</t>
   </si>
   <si>
+    <t>Conservador</t>
+  </si>
+  <si>
     <t>Teste de Procura com:</t>
   </si>
   <si>
@@ -125,9 +128,6 @@
   </si>
   <si>
     <t>Moderado-TIJOLO</t>
-  </si>
-  <si>
-    <t>Moderado</t>
   </si>
   <si>
     <t>Agressivo</t>
@@ -140,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$R$ -416]#,##0.00"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -222,8 +222,8 @@
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
-      <color rgb="FF9C5700"/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
       <name val="Verdana"/>
       <scheme val="minor"/>
     </font>
@@ -231,6 +231,13 @@
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14.0"/>
+      <color rgb="FF9C5700"/>
+      <name val="Verdana"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -328,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border/>
     <border>
       <left style="thick">
@@ -646,6 +653,17 @@
       </bottom>
     </border>
     <border>
+      <left style="hair">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
@@ -654,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -758,76 +776,85 @@
     <xf borderId="27" fillId="2" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="28" fillId="2" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="17" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="6" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="18" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="18" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="19" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="7" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="20" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="21" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="20" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="21" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="20" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="21" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="7" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="22" numFmtId="9" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="9" fontId="23" numFmtId="9" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="28" fillId="0" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="28" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="29" fillId="0" fontId="23" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="29" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="28" fillId="9" fontId="22" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="29" fillId="9" fontId="23" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="22" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="23" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="22" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="4" fontId="23" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="28" fillId="0" fontId="22" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="29" fillId="0" fontId="23" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -907,12 +934,12 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>controle_de_investimentos!$B$29:$B$34</c:f>
+              <c:f>controle_de_investimentos!$B$31:$B$36</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>controle_de_investimentos!$C$29:$C$34</c:f>
+              <c:f>controle_de_investimentos!$C$31:$C$36</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -964,7 +991,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="10791825" cy="4029075"/>
@@ -2129,7 +2156,7 @@
         <f t="shared" si="1"/>
         <v>432216.9655</v>
       </c>
-      <c r="D24" s="36">
+      <c r="D24" s="41">
         <f>$C24*rendimento_carteira</f>
         <v>2593.301793</v>
       </c>
@@ -2159,18 +2186,14 @@
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
     </row>
-    <row r="25" ht="21.0" customHeight="1">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="3"/>
-      <c r="B25" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="42"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="43"/>
+      <c r="G25" s="44"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
@@ -2194,18 +2217,14 @@
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
     </row>
-    <row r="26" ht="18.75" customHeight="1">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3"/>
-      <c r="B26" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="45">
-        <f>aporte</f>
-        <v>100</v>
-      </c>
+      <c r="B26" s="42"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="G26" s="44"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
@@ -2229,14 +2248,18 @@
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" ht="21.0" customHeight="1">
       <c r="A27" s="3"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="46"/>
+      <c r="B27" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="46" t="s">
+        <v>18</v>
+      </c>
       <c r="D27" s="46"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="G27" s="44"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
@@ -2260,16 +2283,14 @@
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
     </row>
-    <row r="28" ht="21.0" customHeight="1">
+    <row r="28" ht="18.75" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
-      <c r="C28" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="47" t="s">
-        <v>22</v>
+      <c r="C28" s="48">
+        <f>aporte</f>
+        <v>100</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -2297,19 +2318,11 @@
       <c r="AB28" s="3"/>
       <c r="AC28" s="3"/>
     </row>
-    <row r="29" ht="18.75" customHeight="1">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3"/>
-      <c r="B29" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="49">
-        <f>VLOOKUP($C$25&amp;"-"&amp;B29,planilha_auxiliar!B3:E21,4,FALSE)</f>
-        <v>0.3</v>
-      </c>
-      <c r="D29" s="50">
-        <f t="shared" ref="D29:D34" si="2">$C29*$C$26</f>
-        <v>30</v>
-      </c>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -2336,18 +2349,16 @@
       <c r="AB29" s="3"/>
       <c r="AC29" s="3"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" ht="21.0" customHeight="1">
       <c r="A30" s="3"/>
-      <c r="B30" s="48" t="s">
-        <v>24</v>
+      <c r="B30" s="50" t="s">
+        <v>20</v>
       </c>
-      <c r="C30" s="49">
-        <f>VLOOKUP($C$25&amp;"-"&amp;B30,planilha_auxiliar!B4:E22,4,FALSE)</f>
-        <v>0.5</v>
+      <c r="C30" s="50" t="s">
+        <v>21</v>
       </c>
-      <c r="D30" s="50">
-        <f t="shared" si="2"/>
-        <v>50</v>
+      <c r="D30" s="50" t="s">
+        <v>22</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -2375,18 +2386,18 @@
       <c r="AB30" s="3"/>
       <c r="AC30" s="3"/>
     </row>
-    <row r="31">
+    <row r="31" ht="18.75" customHeight="1">
       <c r="A31" s="3"/>
-      <c r="B31" s="48" t="s">
-        <v>25</v>
+      <c r="B31" s="51" t="s">
+        <v>23</v>
       </c>
-      <c r="C31" s="49">
-        <f>VLOOKUP($C$25&amp;"-"&amp;B31,planilha_auxiliar!B5:E23,4,FALSE)</f>
-        <v>0.1</v>
+      <c r="C31" s="52">
+        <f>VLOOKUP($C$27&amp;"-"&amp;B31,planilha_auxiliar!B3:E21,4,FALSE)</f>
+        <v>0.32</v>
       </c>
-      <c r="D31" s="50">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="D31" s="53">
+        <f t="shared" ref="D31:D36" si="2">$C31*$C$28</f>
+        <v>32</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -2414,18 +2425,18 @@
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
     </row>
-    <row r="32">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="3"/>
-      <c r="B32" s="48" t="s">
-        <v>26</v>
+      <c r="B32" s="51" t="s">
+        <v>24</v>
       </c>
-      <c r="C32" s="49">
-        <f>VLOOKUP($C$25&amp;"-"&amp;B32,planilha_auxiliar!B6:E24,4,FALSE)</f>
-        <v>0.1</v>
+      <c r="C32" s="52">
+        <f>VLOOKUP($C$27&amp;"-"&amp;B32,planilha_auxiliar!B4:E22,4,FALSE)</f>
+        <v>0.35</v>
       </c>
-      <c r="D32" s="50">
+      <c r="D32" s="53">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -2455,16 +2466,16 @@
     </row>
     <row r="33">
       <c r="A33" s="3"/>
-      <c r="B33" s="48" t="s">
-        <v>27</v>
+      <c r="B33" s="51" t="s">
+        <v>25</v>
       </c>
-      <c r="C33" s="49">
-        <f>VLOOKUP($C$25&amp;"-"&amp;B33,planilha_auxiliar!B7:E25,4,FALSE)</f>
-        <v>0</v>
+      <c r="C33" s="52">
+        <f>VLOOKUP($C$27&amp;"-"&amp;B33,planilha_auxiliar!B5:E23,4,FALSE)</f>
+        <v>0.08</v>
       </c>
-      <c r="D33" s="50">
+      <c r="D33" s="53">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -2494,16 +2505,16 @@
     </row>
     <row r="34">
       <c r="A34" s="3"/>
-      <c r="B34" s="48" t="s">
-        <v>28</v>
+      <c r="B34" s="51" t="s">
+        <v>26</v>
       </c>
-      <c r="C34" s="49">
-        <f>VLOOKUP($C$25&amp;"-"&amp;B34,planilha_auxiliar!B8:E26,4,FALSE)</f>
-        <v>0</v>
+      <c r="C34" s="52">
+        <f>VLOOKUP($C$27&amp;"-"&amp;B34,planilha_auxiliar!B6:E24,4,FALSE)</f>
+        <v>0.05</v>
       </c>
-      <c r="D34" s="50">
+      <c r="D34" s="53">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -2533,11 +2544,16 @@
     </row>
     <row r="35">
       <c r="A35" s="3"/>
-      <c r="B35" s="51"/>
-      <c r="C35" s="52"/>
+      <c r="B35" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="52">
+        <f>VLOOKUP($C$27&amp;"-"&amp;B35,planilha_auxiliar!B7:E25,4,FALSE)</f>
+        <v>0.1</v>
+      </c>
       <c r="D35" s="53">
-        <f>SUM(D29:D34)</f>
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -2567,9 +2583,17 @@
     </row>
     <row r="36">
       <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="B36" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="52">
+        <f>VLOOKUP($C$27&amp;"-"&amp;B36,planilha_auxiliar!B8:E26,4,FALSE)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D36" s="53">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -2598,9 +2622,12 @@
     </row>
     <row r="37">
       <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="56">
+        <f>SUM(D31:D36)</f>
+        <v>100</v>
+      </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -32790,8 +32817,75 @@
       <c r="AB1010" s="3"/>
       <c r="AC1010" s="3"/>
     </row>
+    <row r="1011">
+      <c r="A1011" s="3"/>
+      <c r="B1011" s="3"/>
+      <c r="C1011" s="3"/>
+      <c r="D1011" s="3"/>
+      <c r="E1011" s="3"/>
+      <c r="F1011" s="3"/>
+      <c r="G1011" s="3"/>
+      <c r="H1011" s="3"/>
+      <c r="I1011" s="3"/>
+      <c r="J1011" s="3"/>
+      <c r="K1011" s="3"/>
+      <c r="L1011" s="3"/>
+      <c r="M1011" s="3"/>
+      <c r="N1011" s="3"/>
+      <c r="O1011" s="3"/>
+      <c r="P1011" s="3"/>
+      <c r="Q1011" s="3"/>
+      <c r="R1011" s="3"/>
+      <c r="S1011" s="3"/>
+      <c r="T1011" s="3"/>
+      <c r="U1011" s="3"/>
+      <c r="V1011" s="3"/>
+      <c r="W1011" s="3"/>
+      <c r="X1011" s="3"/>
+      <c r="Y1011" s="3"/>
+      <c r="Z1011" s="3"/>
+      <c r="AA1011" s="3"/>
+      <c r="AB1011" s="3"/>
+      <c r="AC1011" s="3"/>
+    </row>
+    <row r="1012">
+      <c r="A1012" s="3"/>
+      <c r="B1012" s="3"/>
+      <c r="C1012" s="3"/>
+      <c r="D1012" s="3"/>
+      <c r="E1012" s="3"/>
+      <c r="F1012" s="3"/>
+      <c r="G1012" s="3"/>
+      <c r="H1012" s="3"/>
+      <c r="I1012" s="3"/>
+      <c r="J1012" s="3"/>
+      <c r="K1012" s="3"/>
+      <c r="L1012" s="3"/>
+      <c r="M1012" s="3"/>
+      <c r="N1012" s="3"/>
+      <c r="O1012" s="3"/>
+      <c r="P1012" s="3"/>
+      <c r="Q1012" s="3"/>
+      <c r="R1012" s="3"/>
+      <c r="S1012" s="3"/>
+      <c r="T1012" s="3"/>
+      <c r="U1012" s="3"/>
+      <c r="V1012" s="3"/>
+      <c r="W1012" s="3"/>
+      <c r="X1012" s="3"/>
+      <c r="Y1012" s="3"/>
+      <c r="Z1012" s="3"/>
+      <c r="AA1012" s="3"/>
+      <c r="AB1012" s="3"/>
+      <c r="AC1012" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
@@ -32799,14 +32893,9 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C25">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C27">
       <formula1>"Conservador,Moderado,Agressivo"</formula1>
     </dataValidation>
   </dataValidations>
@@ -32831,299 +32920,299 @@
   </cols>
   <sheetData>
     <row r="3">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="57" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="55" t="str">
+      <c r="B4" s="58" t="str">
         <f t="shared" ref="B4:B21" si="1">C4&amp;"-"&amp;D4</f>
         <v>Conservador-PAPEL</v>
       </c>
-      <c r="C4" s="56" t="s">
-        <v>18</v>
+      <c r="C4" s="59" t="s">
+        <v>32</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="57">
+      <c r="E4" s="60">
         <v>0.3</v>
       </c>
-      <c r="G4" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="58" t="s">
+      <c r="G4" s="61" t="s">
         <v>33</v>
       </c>
+      <c r="H4" s="61" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5">
-      <c r="B5" s="55" t="str">
+      <c r="B5" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Conservador-TIJOLO</v>
       </c>
-      <c r="C5" s="56" t="s">
-        <v>18</v>
+      <c r="C5" s="59" t="s">
+        <v>32</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="57">
+      <c r="E5" s="60">
         <v>0.5</v>
       </c>
-      <c r="G5" s="59" t="s">
-        <v>34</v>
+      <c r="G5" s="62" t="s">
+        <v>35</v>
       </c>
-      <c r="H5" s="60">
+      <c r="H5" s="63">
         <f>VLOOKUP(G5,$B3:$E21,4,FALSE())</f>
         <v>0.35</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="55" t="str">
+      <c r="B6" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Conservador-HÍBRIDOS</v>
       </c>
-      <c r="C6" s="56" t="s">
-        <v>18</v>
+      <c r="C6" s="59" t="s">
+        <v>32</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="57">
+      <c r="E6" s="60">
         <v>0.1</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="55" t="str">
+      <c r="B7" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Conservador-FOFs</v>
       </c>
-      <c r="C7" s="56" t="s">
-        <v>18</v>
+      <c r="C7" s="59" t="s">
+        <v>32</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="57">
+      <c r="E7" s="60">
         <v>0.1</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="55" t="str">
+      <c r="B8" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Conservador-DESENVOLVIMENTO</v>
       </c>
-      <c r="C8" s="56" t="s">
-        <v>18</v>
+      <c r="C8" s="59" t="s">
+        <v>32</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="57">
+      <c r="E8" s="60">
         <v>0.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="61" t="str">
+      <c r="B9" s="64" t="str">
         <f t="shared" si="1"/>
         <v>Conservador-HOTELARIA</v>
       </c>
-      <c r="C9" s="62" t="s">
-        <v>18</v>
+      <c r="C9" s="65" t="s">
+        <v>32</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="63">
+      <c r="E9" s="66">
         <v>0.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="55" t="str">
+      <c r="B10" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Moderado-PAPEL</v>
       </c>
-      <c r="C10" s="56" t="s">
-        <v>35</v>
+      <c r="C10" s="59" t="s">
+        <v>18</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="67">
         <v>0.32</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="65" t="str">
+      <c r="B11" s="68" t="str">
         <f t="shared" si="1"/>
         <v>Moderado-TIJOLO</v>
       </c>
-      <c r="C11" s="66" t="s">
-        <v>35</v>
+      <c r="C11" s="69" t="s">
+        <v>18</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="67">
+      <c r="E11" s="70">
         <v>0.35</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="55" t="str">
+      <c r="B12" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Moderado-HÍBRIDOS</v>
       </c>
-      <c r="C12" s="56" t="s">
-        <v>35</v>
+      <c r="C12" s="59" t="s">
+        <v>18</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="64">
+      <c r="E12" s="67">
         <v>0.08</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="55" t="str">
+      <c r="B13" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Moderado-FOFs</v>
       </c>
-      <c r="C13" s="56" t="s">
-        <v>35</v>
+      <c r="C13" s="59" t="s">
+        <v>18</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="67">
         <v>0.05</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="55" t="str">
+      <c r="B14" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Moderado-DESENVOLVIMENTO</v>
       </c>
-      <c r="C14" s="56" t="s">
-        <v>35</v>
+      <c r="C14" s="59" t="s">
+        <v>18</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="67">
         <v>0.1</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="61" t="str">
+      <c r="B15" s="64" t="str">
         <f t="shared" si="1"/>
         <v>Moderado-HOTELARIA</v>
       </c>
-      <c r="C15" s="62" t="s">
-        <v>35</v>
+      <c r="C15" s="65" t="s">
+        <v>18</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="68">
+      <c r="E15" s="71">
         <v>0.1</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="55" t="str">
+      <c r="B16" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Agressivo-PAPEL</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="56" t="s">
+      <c r="D16" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="64">
+      <c r="E16" s="67">
         <v>0.5</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="55" t="str">
+      <c r="B17" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Agressivo-TIJOLO</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="64">
+      <c r="E17" s="67">
         <v>0.1</v>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="55" t="str">
+      <c r="B18" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Agressivo-HÍBRIDOS</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="64">
+      <c r="E18" s="67">
         <v>0.05</v>
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="55" t="str">
+      <c r="B19" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Agressivo-FOFs</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="56" t="s">
+      <c r="D19" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="64">
+      <c r="E19" s="67">
         <v>0.05</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="55" t="str">
+      <c r="B20" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Agressivo-DESENVOLVIMENTO</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="64">
+      <c r="E20" s="67">
         <v>0.2</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="55" t="str">
+      <c r="B21" s="58" t="str">
         <f t="shared" si="1"/>
         <v>Agressivo-HOTELARIA</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="56" t="s">
+      <c r="D21" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="64">
+      <c r="E21" s="67">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>